<commit_message>
minor fixed issue: add category for urb_deg_birth at category tab in non-repeated dictionary “ 
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_2/1_2_non_rep.xlsx
+++ b/dictionaries/urban_ath/1_2/1_2_non_rep.xlsx
@@ -1,47 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\ATHLETE\DOCUMENTS\dictionaries\jose_dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\urban\giovenale\20230927_fixUrbCat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{3C7DCB47-9CAD-40CA-9189-C25A657794B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1966AA9C-8587-4B06-87A8-566EE9436D7B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E6A055-3579-442D-99B6-2499A2848E45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$175</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Categories!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="460">
   <si>
     <t>name</t>
   </si>
@@ -1427,7 +1416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1592,7 +1581,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1704,6 +1693,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1860,7 +1855,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1885,6 +1880,8 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2011,7 +2008,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2309,11 +2306,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMH176"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="26" style="1" customWidth="1"/>
@@ -2321,7 +2318,7 @@
     <col min="5" max="1022" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" s="13" customFormat="1" ht="15">
+    <row r="1" spans="1:1022" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2335,7 +2332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1022" s="8" customFormat="1">
+    <row r="2" spans="1:1022" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2349,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1022" s="8" customFormat="1">
+    <row r="3" spans="1:1022" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +3375,7 @@
       <c r="AMG3" s="9"/>
       <c r="AMH3" s="9"/>
     </row>
-    <row r="4" spans="1:1022" s="8" customFormat="1">
+    <row r="4" spans="1:1022" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -4410,17 +4407,17 @@
       <c r="AMG4" s="9"/>
       <c r="AMH4" s="9"/>
     </row>
-    <row r="5" spans="1:1022" s="8" customFormat="1" ht="15">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:1022" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="9"/>
@@ -5442,17 +5439,17 @@
       <c r="AMG5" s="9"/>
       <c r="AMH5" s="9"/>
     </row>
-    <row r="6" spans="1:1022" s="8" customFormat="1" ht="15">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:1022" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="9"/>
@@ -6474,7 +6471,7 @@
       <c r="AMG6" s="9"/>
       <c r="AMH6" s="9"/>
     </row>
-    <row r="7" spans="1:1022" s="8" customFormat="1">
+    <row r="7" spans="1:1022" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -7506,7 +7503,7 @@
       <c r="AMG7" s="9"/>
       <c r="AMH7" s="9"/>
     </row>
-    <row r="8" spans="1:1022" s="8" customFormat="1">
+    <row r="8" spans="1:1022" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
@@ -8538,7 +8535,7 @@
       <c r="AMG8" s="9"/>
       <c r="AMH8" s="9"/>
     </row>
-    <row r="9" spans="1:1022">
+    <row r="9" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -8550,7 +8547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:1022">
+    <row r="10" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -8562,7 +8559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:1022">
+    <row r="11" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -8576,7 +8573,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1022">
+    <row r="12" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -8590,7 +8587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1022">
+    <row r="13" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -8604,7 +8601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:1022">
+    <row r="14" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -8618,7 +8615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:1022">
+    <row r="15" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -8630,7 +8627,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:1022">
+    <row r="16" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -8644,7 +8641,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -8658,7 +8655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -8672,7 +8669,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -8686,7 +8683,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -8700,7 +8697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -8712,7 +8709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -8726,7 +8723,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -8740,7 +8737,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -8752,7 +8749,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -8766,7 +8763,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -8780,7 +8777,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -8794,7 +8791,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -8808,7 +8805,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -8822,7 +8819,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -8836,7 +8833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -8850,7 +8847,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -8862,7 +8859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -8874,7 +8871,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -8888,7 +8885,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -8902,7 +8899,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -8916,7 +8913,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -8930,7 +8927,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -8944,7 +8941,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -8956,7 +8953,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -8970,7 +8967,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -8984,7 +8981,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -8998,7 +8995,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -9012,7 +9009,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -9026,7 +9023,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -9040,7 +9037,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -9054,7 +9051,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -9068,7 +9065,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -9082,7 +9079,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -9096,7 +9093,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -9110,7 +9107,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>118</v>
       </c>
@@ -9124,7 +9121,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -9138,7 +9135,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -9152,7 +9149,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -9166,7 +9163,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -9180,7 +9177,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -9194,7 +9191,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>131</v>
       </c>
@@ -9208,7 +9205,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -9222,7 +9219,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -9236,7 +9233,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -9250,7 +9247,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -9264,7 +9261,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -9278,7 +9275,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -9292,7 +9289,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -9306,7 +9303,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -9320,7 +9317,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -9334,7 +9331,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -9348,7 +9345,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -9362,7 +9359,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -9376,7 +9373,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -9390,7 +9387,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>160</v>
       </c>
@@ -9404,7 +9401,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -9418,7 +9415,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -9432,7 +9429,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -9446,7 +9443,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -9460,7 +9457,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>170</v>
       </c>
@@ -9474,7 +9471,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>172</v>
       </c>
@@ -9488,7 +9485,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -9502,7 +9499,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -9516,7 +9513,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -9530,7 +9527,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>182</v>
       </c>
@@ -9544,7 +9541,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>184</v>
       </c>
@@ -9558,7 +9555,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>187</v>
       </c>
@@ -9572,7 +9569,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -9586,7 +9583,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -9600,7 +9597,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -9614,7 +9611,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>196</v>
       </c>
@@ -9628,7 +9625,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>198</v>
       </c>
@@ -9642,7 +9639,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>200</v>
       </c>
@@ -9656,7 +9653,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>202</v>
       </c>
@@ -9670,7 +9667,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>204</v>
       </c>
@@ -9684,7 +9681,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>206</v>
       </c>
@@ -9698,7 +9695,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>209</v>
       </c>
@@ -9712,7 +9709,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>211</v>
       </c>
@@ -9726,7 +9723,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>213</v>
       </c>
@@ -9740,7 +9737,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>215</v>
       </c>
@@ -9754,7 +9751,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>217</v>
       </c>
@@ -9768,7 +9765,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>219</v>
       </c>
@@ -9782,7 +9779,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>222</v>
       </c>
@@ -9796,7 +9793,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>224</v>
       </c>
@@ -9810,7 +9807,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>226</v>
       </c>
@@ -9824,7 +9821,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>228</v>
       </c>
@@ -9836,7 +9833,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>230</v>
       </c>
@@ -9850,7 +9847,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>232</v>
       </c>
@@ -9862,7 +9859,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>234</v>
       </c>
@@ -9876,7 +9873,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>236</v>
       </c>
@@ -9890,7 +9887,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>238</v>
       </c>
@@ -9902,7 +9899,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>240</v>
       </c>
@@ -9914,7 +9911,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>242</v>
       </c>
@@ -9928,7 +9925,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>244</v>
       </c>
@@ -9942,7 +9939,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>246</v>
       </c>
@@ -9956,7 +9953,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>248</v>
       </c>
@@ -9970,7 +9967,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>250</v>
       </c>
@@ -9982,7 +9979,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>252</v>
       </c>
@@ -9996,7 +9993,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>254</v>
       </c>
@@ -10010,7 +10007,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>256</v>
       </c>
@@ -10024,7 +10021,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>258</v>
       </c>
@@ -10038,7 +10035,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>260</v>
       </c>
@@ -10052,7 +10049,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>262</v>
       </c>
@@ -10064,7 +10061,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>264</v>
       </c>
@@ -10078,7 +10075,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>266</v>
       </c>
@@ -10092,7 +10089,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>268</v>
       </c>
@@ -10104,7 +10101,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>270</v>
       </c>
@@ -10118,7 +10115,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>272</v>
       </c>
@@ -10132,7 +10129,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>274</v>
       </c>
@@ -10146,7 +10143,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>276</v>
       </c>
@@ -10158,7 +10155,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>278</v>
       </c>
@@ -10170,7 +10167,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>280</v>
       </c>
@@ -10184,7 +10181,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>282</v>
       </c>
@@ -10198,7 +10195,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>284</v>
       </c>
@@ -10212,7 +10209,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>286</v>
       </c>
@@ -10226,7 +10223,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>288</v>
       </c>
@@ -10240,7 +10237,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>290</v>
       </c>
@@ -10252,7 +10249,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>292</v>
       </c>
@@ -10266,7 +10263,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>294</v>
       </c>
@@ -10280,7 +10277,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>296</v>
       </c>
@@ -10294,7 +10291,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>298</v>
       </c>
@@ -10308,7 +10305,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>300</v>
       </c>
@@ -10322,7 +10319,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>302</v>
       </c>
@@ -10336,7 +10333,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>304</v>
       </c>
@@ -10350,7 +10347,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>306</v>
       </c>
@@ -10364,7 +10361,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>308</v>
       </c>
@@ -10378,7 +10375,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>310</v>
       </c>
@@ -10392,7 +10389,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>312</v>
       </c>
@@ -10406,7 +10403,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>314</v>
       </c>
@@ -10420,7 +10417,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>316</v>
       </c>
@@ -10434,7 +10431,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>318</v>
       </c>
@@ -10448,7 +10445,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>320</v>
       </c>
@@ -10462,7 +10459,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>322</v>
       </c>
@@ -10476,7 +10473,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>324</v>
       </c>
@@ -10490,7 +10487,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>326</v>
       </c>
@@ -10504,7 +10501,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>328</v>
       </c>
@@ -10518,7 +10515,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>330</v>
       </c>
@@ -10532,7 +10529,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>332</v>
       </c>
@@ -10546,7 +10543,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>334</v>
       </c>
@@ -10560,7 +10557,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>336</v>
       </c>
@@ -10574,7 +10571,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>338</v>
       </c>
@@ -10588,7 +10585,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>340</v>
       </c>
@@ -10602,7 +10599,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>342</v>
       </c>
@@ -10616,7 +10613,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>344</v>
       </c>
@@ -10630,7 +10627,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>346</v>
       </c>
@@ -10644,7 +10641,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>348</v>
       </c>
@@ -10658,7 +10655,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>351</v>
       </c>
@@ -10672,7 +10669,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>353</v>
       </c>
@@ -10686,7 +10683,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>355</v>
       </c>
@@ -10700,7 +10697,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>357</v>
       </c>
@@ -10714,7 +10711,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>359</v>
       </c>
@@ -10728,7 +10725,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>361</v>
       </c>
@@ -10742,7 +10739,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>363</v>
       </c>
@@ -10756,7 +10753,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>365</v>
       </c>
@@ -10770,7 +10767,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>367</v>
       </c>
@@ -10784,7 +10781,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>369</v>
       </c>
@@ -10798,7 +10795,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>371</v>
       </c>
@@ -10812,7 +10809,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>373</v>
       </c>
@@ -10824,7 +10821,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>375</v>
       </c>
@@ -10838,7 +10835,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C176"/>
     </row>
   </sheetData>
@@ -10856,19 +10853,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:XFD87"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="26" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="15">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>377</v>
       </c>
@@ -10883,7 +10880,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -10897,7 +10894,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -10911,7 +10908,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -10925,7 +10922,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -10939,7 +10936,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -10953,7 +10950,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -10967,7 +10964,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -10981,7 +10978,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -10995,7 +10992,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -11009,7 +11006,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -11023,7 +11020,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -11037,7 +11034,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -11051,7 +11048,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -11065,7 +11062,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -11079,7 +11076,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -11093,7 +11090,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
@@ -11107,7 +11104,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -11121,7 +11118,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -11135,7 +11132,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -11149,7 +11146,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -11163,7 +11160,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
@@ -11177,7 +11174,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
@@ -11191,7 +11188,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -11205,7 +11202,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
@@ -11219,7 +11216,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="26" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
@@ -11233,7 +11230,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
@@ -11247,7 +11244,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -11261,7 +11258,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
@@ -11275,7 +11272,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
@@ -11289,7 +11286,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="31" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>11</v>
       </c>
@@ -11303,7 +11300,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="32" spans="1:4" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>11</v>
       </c>
@@ -11317,7 +11314,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="33" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>11</v>
       </c>
@@ -11331,7 +11328,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="34" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>13</v>
       </c>
@@ -11345,7 +11342,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="35" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>13</v>
       </c>
@@ -11359,7 +11356,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="36" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>13</v>
       </c>
@@ -11373,7 +11370,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="37" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>13</v>
       </c>
@@ -11387,7 +11384,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="38" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>13</v>
       </c>
@@ -11401,7 +11398,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="39" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>13</v>
       </c>
@@ -11415,7 +11412,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="40" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>13</v>
       </c>
@@ -11429,7 +11426,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="8" customFormat="1" ht="15">
+    <row r="41" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
@@ -11443,471 +11440,487 @@
         <v>418</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>232</v>
-      </c>
-      <c r="B42">
-        <v>1001</v>
-      </c>
-      <c r="C42" t="b">
+    <row r="42" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="11">
+        <v>30</v>
+      </c>
+      <c r="C42" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D42" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>232</v>
-      </c>
-      <c r="B43">
-        <v>1102</v>
-      </c>
-      <c r="C43" t="b">
+      <c r="D42" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="11">
+        <v>23</v>
+      </c>
+      <c r="C43" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D43" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>232</v>
-      </c>
-      <c r="B44">
-        <v>1103</v>
-      </c>
-      <c r="C44" t="b">
+      <c r="D43" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="11">
+        <v>22</v>
+      </c>
+      <c r="C44" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D44" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45">
-        <v>1104</v>
-      </c>
-      <c r="C45" t="b">
+      <c r="D44" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="11">
+        <v>21</v>
+      </c>
+      <c r="C45" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D45" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>232</v>
-      </c>
-      <c r="B46">
-        <v>1201</v>
-      </c>
-      <c r="C46" t="b">
+      <c r="D45" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="11">
+        <v>13</v>
+      </c>
+      <c r="C46" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D46" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>232</v>
-      </c>
-      <c r="B47">
-        <v>1202</v>
-      </c>
-      <c r="C47" t="b">
+      <c r="D46" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="11">
+        <v>12</v>
+      </c>
+      <c r="C47" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D47" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>232</v>
-      </c>
-      <c r="B48">
-        <v>1203</v>
-      </c>
-      <c r="C48" t="b">
+      <c r="D47" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="11">
+        <v>11</v>
+      </c>
+      <c r="C48" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D48" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49">
-        <v>1204</v>
-      </c>
-      <c r="C49" t="b">
+      <c r="D48" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="11">
+        <v>10</v>
+      </c>
+      <c r="C49" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D49" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="D49" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>232</v>
       </c>
       <c r="B50">
-        <v>1205</v>
+        <v>1001</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>232</v>
       </c>
       <c r="B51">
-        <v>1301</v>
+        <v>1102</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>232</v>
       </c>
       <c r="B52">
-        <v>1401</v>
+        <v>1103</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>232</v>
       </c>
       <c r="B53">
-        <v>1402</v>
+        <v>1104</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>232</v>
       </c>
       <c r="B54">
-        <v>1403</v>
+        <v>1201</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>232</v>
       </c>
       <c r="B55">
-        <v>1404</v>
+        <v>1202</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>232</v>
       </c>
       <c r="B56">
-        <v>1501</v>
+        <v>1203</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>232</v>
       </c>
       <c r="B57">
-        <v>1601</v>
+        <v>1204</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>232</v>
       </c>
       <c r="B58">
-        <v>1701</v>
+        <v>1205</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>232</v>
       </c>
       <c r="B59">
-        <v>1801</v>
+        <v>1301</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>232</v>
       </c>
       <c r="B60">
-        <v>1802</v>
+        <v>1401</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>232</v>
       </c>
       <c r="B61">
-        <v>1803</v>
+        <v>1402</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>232</v>
       </c>
       <c r="B62">
-        <v>1901</v>
+        <v>1403</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>232</v>
       </c>
       <c r="B63">
-        <v>1804</v>
+        <v>1404</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>232</v>
       </c>
       <c r="B64">
-        <v>2101</v>
+        <v>1501</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>232</v>
       </c>
       <c r="B65">
-        <v>2201</v>
+        <v>1601</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>232</v>
       </c>
       <c r="B66">
+        <v>1701</v>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>232</v>
+      </c>
+      <c r="B67">
+        <v>1801</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>232</v>
+      </c>
+      <c r="B68">
+        <v>1802</v>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69">
+        <v>1803</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>232</v>
+      </c>
+      <c r="B70">
+        <v>1901</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>232</v>
+      </c>
+      <c r="B71">
+        <v>1804</v>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>232</v>
+      </c>
+      <c r="B72">
+        <v>2101</v>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73">
+        <v>2201</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>232</v>
+      </c>
+      <c r="B74">
         <v>2301</v>
-      </c>
-      <c r="C66" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D66" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D67" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>25</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
-      </c>
-      <c r="C68" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>25</v>
-      </c>
-      <c r="B69">
-        <v>3</v>
-      </c>
-      <c r="C69" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D70" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="C71" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D71" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>23</v>
-      </c>
-      <c r="B72">
-        <v>3</v>
-      </c>
-      <c r="C72" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D72" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>23</v>
-      </c>
-      <c r="B73">
-        <v>4</v>
-      </c>
-      <c r="C73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D73" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>23</v>
-      </c>
-      <c r="B74">
-        <v>5</v>
       </c>
       <c r="C74" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -11916,12 +11929,12 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -11930,12 +11943,12 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -11944,264 +11957,264 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C78" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C79" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B80">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C80" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C81" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C82" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B84">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C84" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C85" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B86">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C86" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C87" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>240</v>
+        <v>77</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C91" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C92" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C93" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C94" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>238</v>
+        <v>58</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C95" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -12210,12 +12223,12 @@
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -12224,12 +12237,12 @@
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -12238,406 +12251,518 @@
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C99" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="B100">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C100" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="B101">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C101" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>290</v>
+        <v>238</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C102" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>290</v>
+        <v>238</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C103" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C104" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C105" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C106" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="B107">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C107" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C108" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C109" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>38</v>
-      </c>
-      <c r="B110" s="1">
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
       </c>
       <c r="C110" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>38</v>
-      </c>
-      <c r="B111" s="1">
-        <v>1</v>
+        <v>290</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
       </c>
       <c r="C111" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>58</v>
-      </c>
-      <c r="B112" s="1">
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="B112">
+        <v>3</v>
       </c>
       <c r="C112" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>250</v>
-      </c>
-      <c r="B113" s="1">
-        <v>1</v>
+        <v>290</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
       </c>
       <c r="C113" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>268</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="B114">
+        <v>5</v>
       </c>
       <c r="C114" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D114" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>290</v>
+      </c>
+      <c r="B115">
+        <v>6</v>
+      </c>
+      <c r="C115" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D115" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>250</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D116" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>268</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D117" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>38</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0</v>
+      </c>
+      <c r="C118" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D118" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>38</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1</v>
+      </c>
+      <c r="C119" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D119" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>58</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0</v>
+      </c>
+      <c r="C120" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D120" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>250</v>
+      </c>
+      <c r="B121" s="1">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D121" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>268</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0</v>
+      </c>
+      <c r="C122" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D122" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B128" s="1"/>
     </row>
-    <row r="129" spans="2:2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" s="1"/>
     </row>
-    <row r="130" spans="2:2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="2:2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="2:2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="2:2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" s="1"/>
     </row>
-    <row r="134" spans="2:2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" s="1"/>
     </row>
-    <row r="135" spans="2:2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" s="1"/>
     </row>
-    <row r="136" spans="2:2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="2:2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" s="1"/>
     </row>
-    <row r="138" spans="2:2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:2">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:2">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" s="1"/>
     </row>
-    <row r="145" spans="2:2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" s="1"/>
     </row>
-    <row r="146" spans="2:2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="2:2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" s="1"/>
     </row>
-    <row r="148" spans="2:2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="2:2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="2:2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="1"/>
     </row>
-    <row r="151" spans="2:2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="2:2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="1"/>
     </row>
-    <row r="153" spans="2:2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" s="1"/>
     </row>
-    <row r="154" spans="2:2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="1"/>
     </row>
-    <row r="155" spans="2:2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="1"/>
     </row>
-    <row r="156" spans="2:2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="2:2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" s="1"/>
     </row>
-    <row r="158" spans="2:2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="2:2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" s="1"/>
     </row>
-    <row r="160" spans="2:2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" s="1"/>
     </row>
-    <row r="161" spans="2:2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" s="1"/>
     </row>
-    <row r="162" spans="2:2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" s="1"/>
     </row>
-    <row r="163" spans="2:2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" s="1"/>
     </row>
-    <row r="164" spans="2:2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" s="1"/>
     </row>
-    <row r="165" spans="2:2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" s="1"/>
     </row>
-    <row r="166" spans="2:2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" s="1"/>
     </row>
-    <row r="167" spans="2:2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" s="1"/>
     </row>
-    <row r="168" spans="2:2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" s="1"/>
     </row>
-    <row r="169" spans="2:2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" s="1"/>
     </row>
-    <row r="170" spans="2:2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" s="1"/>
     </row>
-    <row r="171" spans="2:2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" s="1"/>
     </row>
-    <row r="172" spans="2:2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B180" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>

</xml_diff>